<commit_message>
Updated spreadsheet for summer 2017
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2017summer.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2017summer.xlsx
@@ -15,7 +15,7 @@
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -732,6 +732,9 @@
   <si>
     <t>2017 sum
 Alina</t>
+  </si>
+  <si>
+    <t>Using iPads</t>
   </si>
 </sst>
 </file>
@@ -1946,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y110"/>
+  <dimension ref="A1:Y111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P66" sqref="P66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2057,7 +2060,9 @@
         <v>1</v>
       </c>
       <c r="N2" s="59"/>
-      <c r="O2" s="55"/>
+      <c r="O2" s="55">
+        <v>1</v>
+      </c>
       <c r="P2" s="75">
         <f>SUM(J2:M2)</f>
         <v>3</v>
@@ -2099,9 +2104,11 @@
         <v>1</v>
       </c>
       <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
+      <c r="O3" s="60">
+        <v>1</v>
+      </c>
       <c r="P3" s="76">
-        <f t="shared" ref="P3:P66" si="0">SUM(J3:M3)</f>
+        <f t="shared" ref="P3:P67" si="0">SUM(J3:M3)</f>
         <v>3</v>
       </c>
       <c r="Q3" s="80"/>
@@ -2147,7 +2154,9 @@
         <v>0.5</v>
       </c>
       <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
+      <c r="O4" s="36">
+        <v>1</v>
+      </c>
       <c r="P4" s="77">
         <f t="shared" si="0"/>
         <v>2.5</v>
@@ -2307,7 +2316,9 @@
       <c r="M9" s="2">
         <v>1</v>
       </c>
-      <c r="O9" s="34"/>
+      <c r="O9" s="34">
+        <v>1</v>
+      </c>
       <c r="P9" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2352,7 +2363,9 @@
         <v>1</v>
       </c>
       <c r="N10" s="36"/>
-      <c r="O10" s="34"/>
+      <c r="O10" s="34">
+        <v>1</v>
+      </c>
       <c r="P10" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2394,7 +2407,9 @@
         <v>0.75</v>
       </c>
       <c r="N11" s="36"/>
-      <c r="O11" s="34"/>
+      <c r="O11" s="34">
+        <v>1</v>
+      </c>
       <c r="P11" s="77">
         <f t="shared" si="0"/>
         <v>2.25</v>
@@ -2471,7 +2486,9 @@
         <v>1</v>
       </c>
       <c r="N13" s="36"/>
-      <c r="O13" s="34"/>
+      <c r="O13" s="34">
+        <v>1</v>
+      </c>
       <c r="P13" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2513,7 +2530,9 @@
         <v>0.5</v>
       </c>
       <c r="N14" s="36"/>
-      <c r="O14" s="34"/>
+      <c r="O14" s="34">
+        <v>1</v>
+      </c>
       <c r="P14" s="77">
         <f t="shared" si="0"/>
         <v>2.5</v>
@@ -2666,7 +2685,9 @@
         <v>0.75</v>
       </c>
       <c r="N18" s="36"/>
-      <c r="O18" s="34"/>
+      <c r="O18" s="34">
+        <v>1</v>
+      </c>
       <c r="P18" s="77">
         <f t="shared" si="0"/>
         <v>3.75</v>
@@ -2828,15 +2849,15 @@
         <v>0</v>
       </c>
       <c r="S23" s="6">
-        <f t="shared" ref="S23:S31" si="1">SUMIF(P$2:P$68,"&gt;=" &amp; R23,C$2:C$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R23,C$2:C$69)</f>
         <v>296</v>
       </c>
       <c r="T23" s="6">
-        <f t="shared" ref="T23:T31" si="2">SUMIF(P$2:P$68,"&gt;=" &amp; R23,D$2:D$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R23,D$2:D$69)</f>
         <v>7</v>
       </c>
       <c r="U23" s="8">
-        <f t="shared" ref="U23:U31" si="3">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
+        <f t="shared" ref="U23:U31" si="1">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
         <v>25.870000000000005</v>
       </c>
       <c r="V23" s="33"/>
@@ -2877,7 +2898,9 @@
         <v>1</v>
       </c>
       <c r="N24" s="20"/>
-      <c r="O24" s="34"/>
+      <c r="O24" s="34">
+        <v>1</v>
+      </c>
       <c r="P24" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2887,15 +2910,15 @@
         <v>0.5</v>
       </c>
       <c r="S24" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R24,C$2:C$69)</f>
+        <v>270</v>
+      </c>
+      <c r="T24" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R24,D$2:D$69)</f>
+        <v>7</v>
+      </c>
+      <c r="U24" s="8">
         <f t="shared" si="1"/>
-        <v>270</v>
-      </c>
-      <c r="T24" s="6">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="U24" s="8">
-        <f t="shared" si="3"/>
         <v>24.180000000000003</v>
       </c>
       <c r="V24" s="33"/>
@@ -2919,7 +2942,9 @@
       <c r="M25" s="2">
         <v>0</v>
       </c>
-      <c r="O25" s="34"/>
+      <c r="O25" s="34">
+        <v>1</v>
+      </c>
       <c r="P25" s="77">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2929,15 +2954,15 @@
         <v>1</v>
       </c>
       <c r="S25" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R25,C$2:C$69)</f>
+        <v>246</v>
+      </c>
+      <c r="T25" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R25,D$2:D$69)</f>
+        <v>7</v>
+      </c>
+      <c r="U25" s="8">
         <f t="shared" si="1"/>
-        <v>246</v>
-      </c>
-      <c r="T25" s="6">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="U25" s="8">
-        <f t="shared" si="3"/>
         <v>22.620000000000005</v>
       </c>
       <c r="V25" s="33"/>
@@ -2971,7 +2996,9 @@
       <c r="M26" s="2">
         <v>1</v>
       </c>
-      <c r="O26" s="34"/>
+      <c r="O26" s="34">
+        <v>1</v>
+      </c>
       <c r="P26" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2981,15 +3008,15 @@
         <v>1.5</v>
       </c>
       <c r="S26" s="31">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R26,C$2:C$69)</f>
+        <v>211</v>
+      </c>
+      <c r="T26" s="31">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R26,D$2:D$69)</f>
+        <v>6</v>
+      </c>
+      <c r="U26" s="8">
         <f t="shared" si="1"/>
-        <v>211</v>
-      </c>
-      <c r="T26" s="31">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="U26" s="8">
-        <f t="shared" si="3"/>
         <v>19.955000000000002</v>
       </c>
       <c r="V26" s="33"/>
@@ -3032,7 +3059,9 @@
         <v>1</v>
       </c>
       <c r="N27" s="12"/>
-      <c r="O27" s="35"/>
+      <c r="O27" s="35">
+        <v>1</v>
+      </c>
       <c r="P27" s="78">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -3042,15 +3071,15 @@
         <v>2</v>
       </c>
       <c r="S27" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R27,C$2:C$69)</f>
+        <v>180</v>
+      </c>
+      <c r="T27" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R27,D$2:D$69)</f>
+        <v>6</v>
+      </c>
+      <c r="U27" s="8">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="T27" s="6">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="U27" s="8">
-        <f t="shared" si="3"/>
         <v>17.940000000000001</v>
       </c>
     </row>
@@ -3077,7 +3106,9 @@
       <c r="M28" s="2">
         <v>0.8</v>
       </c>
-      <c r="O28" s="34"/>
+      <c r="O28" s="34">
+        <v>1</v>
+      </c>
       <c r="P28" s="77">
         <f t="shared" si="0"/>
         <v>1.8</v>
@@ -3087,15 +3118,15 @@
         <v>2.5</v>
       </c>
       <c r="S28" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R28,C$2:C$69)</f>
+        <v>156</v>
+      </c>
+      <c r="T28" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R28,D$2:D$69)</f>
+        <v>1</v>
+      </c>
+      <c r="U28" s="8">
         <f t="shared" si="1"/>
-        <v>156</v>
-      </c>
-      <c r="T28" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="U28" s="8">
-        <f t="shared" si="3"/>
         <v>14.430000000000001</v>
       </c>
     </row>
@@ -3123,15 +3154,15 @@
         <v>3</v>
       </c>
       <c r="S29" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R29,C$2:C$69)</f>
+        <v>129</v>
+      </c>
+      <c r="T29" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R29,D$2:D$69)</f>
+        <v>1</v>
+      </c>
+      <c r="U29" s="8">
         <f t="shared" si="1"/>
-        <v>129</v>
-      </c>
-      <c r="T29" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="U29" s="8">
-        <f t="shared" si="3"/>
         <v>12.675000000000001</v>
       </c>
     </row>
@@ -3160,7 +3191,9 @@
         <v>0.5</v>
       </c>
       <c r="N30" s="36"/>
-      <c r="O30" s="34"/>
+      <c r="O30" s="34">
+        <v>1</v>
+      </c>
       <c r="P30" s="77">
         <f t="shared" si="0"/>
         <v>1.5</v>
@@ -3170,15 +3203,15 @@
         <v>3.5</v>
       </c>
       <c r="S30" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R30,C$2:C$69)</f>
+        <v>81</v>
+      </c>
+      <c r="T30" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R30,D$2:D$69)</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="8">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="T30" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U30" s="8">
-        <f t="shared" si="3"/>
         <v>9.1650000000000009</v>
       </c>
     </row>
@@ -3212,7 +3245,9 @@
         <v>0.5</v>
       </c>
       <c r="N31" s="36"/>
-      <c r="O31" s="34"/>
+      <c r="O31" s="34">
+        <v>1</v>
+      </c>
       <c r="P31" s="77">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -3222,15 +3257,15 @@
         <v>4</v>
       </c>
       <c r="S31" s="47">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R31,C$2:C$69)</f>
+        <v>47</v>
+      </c>
+      <c r="T31" s="47">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R31,D$2:D$69)</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="9">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="T31" s="47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U31" s="9">
-        <f t="shared" si="3"/>
         <v>6.9550000000000001</v>
       </c>
     </row>
@@ -3295,7 +3330,9 @@
         <v>0.5</v>
       </c>
       <c r="N33" s="36"/>
-      <c r="O33" s="34"/>
+      <c r="O33" s="34">
+        <v>1</v>
+      </c>
       <c r="P33" s="77">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -3320,7 +3357,9 @@
         <v>0.5</v>
       </c>
       <c r="N34" s="36"/>
-      <c r="O34" s="34"/>
+      <c r="O34" s="34">
+        <v>1</v>
+      </c>
       <c r="P34" s="77">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3354,7 +3393,9 @@
         <v>1</v>
       </c>
       <c r="N35" s="36"/>
-      <c r="O35" s="34"/>
+      <c r="O35" s="34">
+        <v>1</v>
+      </c>
       <c r="P35" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3386,7 +3427,9 @@
         <v>0.5</v>
       </c>
       <c r="N36" s="36"/>
-      <c r="O36" s="34"/>
+      <c r="O36" s="34">
+        <v>1</v>
+      </c>
       <c r="P36" s="77">
         <f t="shared" si="0"/>
         <v>1.5</v>
@@ -3417,7 +3460,9 @@
       <c r="M37" s="2">
         <v>0.8</v>
       </c>
-      <c r="O37" s="34"/>
+      <c r="O37" s="34">
+        <v>1</v>
+      </c>
       <c r="P37" s="77">
         <f t="shared" si="0"/>
         <v>1.8</v>
@@ -3461,7 +3506,9 @@
         <v>1</v>
       </c>
       <c r="N38" s="12"/>
-      <c r="O38" s="35"/>
+      <c r="O38" s="35">
+        <v>1</v>
+      </c>
       <c r="P38" s="78">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3496,7 +3543,9 @@
         <v>0.75</v>
       </c>
       <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
+      <c r="O39" s="36">
+        <v>1</v>
+      </c>
       <c r="P39" s="77">
         <f t="shared" si="0"/>
         <v>2.75</v>
@@ -3538,7 +3587,9 @@
         <v>0.5</v>
       </c>
       <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
+      <c r="O40" s="36">
+        <v>1</v>
+      </c>
       <c r="P40" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3611,7 +3662,9 @@
         <v>0</v>
       </c>
       <c r="N42" s="36"/>
-      <c r="O42" s="36"/>
+      <c r="O42" s="36">
+        <v>1</v>
+      </c>
       <c r="P42" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3647,7 +3700,9 @@
         <v>1</v>
       </c>
       <c r="N43" s="36"/>
-      <c r="O43" s="36"/>
+      <c r="O43" s="36">
+        <v>1</v>
+      </c>
       <c r="P43" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3684,7 +3739,9 @@
         <v>0.75</v>
       </c>
       <c r="N44" s="36"/>
-      <c r="O44" s="36"/>
+      <c r="O44" s="36">
+        <v>1</v>
+      </c>
       <c r="P44" s="77">
         <f t="shared" si="0"/>
         <v>2.75</v>
@@ -3725,7 +3782,9 @@
         <v>1</v>
       </c>
       <c r="N45" s="36"/>
-      <c r="O45" s="36"/>
+      <c r="O45" s="36">
+        <v>1</v>
+      </c>
       <c r="P45" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3769,7 +3828,9 @@
         <v>0</v>
       </c>
       <c r="N46" s="36"/>
-      <c r="O46" s="36"/>
+      <c r="O46" s="36">
+        <v>1</v>
+      </c>
       <c r="P46" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3805,7 +3866,9 @@
       <c r="M47" s="2">
         <v>1</v>
       </c>
-      <c r="O47" s="34"/>
+      <c r="O47" s="34">
+        <v>1</v>
+      </c>
       <c r="P47" s="77">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3845,7 +3908,9 @@
         <v>0</v>
       </c>
       <c r="N48" s="12"/>
-      <c r="O48" s="35"/>
+      <c r="O48" s="35">
+        <v>1</v>
+      </c>
       <c r="P48" s="78">
         <f t="shared" si="0"/>
         <v>1.5</v>
@@ -3887,7 +3952,9 @@
       <c r="M49" s="2">
         <v>0.7</v>
       </c>
-      <c r="O49" s="34"/>
+      <c r="O49" s="34">
+        <v>1</v>
+      </c>
       <c r="P49" s="77">
         <f t="shared" si="0"/>
         <v>3.7</v>
@@ -3931,7 +3998,9 @@
         <v>1</v>
       </c>
       <c r="N50" s="20"/>
-      <c r="O50" s="34"/>
+      <c r="O50" s="34">
+        <v>1</v>
+      </c>
       <c r="P50" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4042,7 +4111,9 @@
       <c r="M54" s="2">
         <v>1</v>
       </c>
-      <c r="O54" s="34"/>
+      <c r="O54" s="34">
+        <v>1</v>
+      </c>
       <c r="P54" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4081,7 +4152,9 @@
         <v>1</v>
       </c>
       <c r="N55" s="12"/>
-      <c r="O55" s="35"/>
+      <c r="O55" s="35">
+        <v>1</v>
+      </c>
       <c r="P55" s="78">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4119,7 +4192,9 @@
       <c r="M56" s="2">
         <v>1</v>
       </c>
-      <c r="O56" s="34"/>
+      <c r="O56" s="34">
+        <v>1</v>
+      </c>
       <c r="P56" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4156,7 +4231,9 @@
       <c r="M57" s="2">
         <v>1</v>
       </c>
-      <c r="O57" s="34"/>
+      <c r="O57" s="34">
+        <v>1</v>
+      </c>
       <c r="P57" s="77">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4274,7 +4351,9 @@
         <v>1</v>
       </c>
       <c r="N61" s="12"/>
-      <c r="O61" s="35"/>
+      <c r="O61" s="35">
+        <v>1</v>
+      </c>
       <c r="P61" s="78">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4297,7 +4376,9 @@
       <c r="M62" s="20">
         <v>1</v>
       </c>
-      <c r="O62" s="36"/>
+      <c r="O62" s="36">
+        <v>1</v>
+      </c>
       <c r="P62" s="77">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4329,7 +4410,9 @@
         <v>1</v>
       </c>
       <c r="N63" s="20"/>
-      <c r="O63" s="34"/>
+      <c r="O63" s="34">
+        <v>0</v>
+      </c>
       <c r="P63" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4361,7 +4444,9 @@
       <c r="M64" s="2">
         <v>1</v>
       </c>
-      <c r="O64" s="34"/>
+      <c r="O64" s="34">
+        <v>1</v>
+      </c>
       <c r="P64" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4389,7 +4474,9 @@
       <c r="M65" s="2">
         <v>0</v>
       </c>
-      <c r="O65" s="34"/>
+      <c r="O65" s="34">
+        <v>1</v>
+      </c>
       <c r="P65" s="77">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4417,244 +4504,264 @@
       <c r="M66" s="2">
         <v>1</v>
       </c>
-      <c r="O66" s="34"/>
+      <c r="O66" s="34">
+        <v>1</v>
+      </c>
       <c r="P66" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q66" s="15"/>
     </row>
-    <row r="67" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
-      <c r="B67" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="27">
-        <v>4</v>
-      </c>
-      <c r="D67" s="27">
+      <c r="B67" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="34"/>
+      <c r="M67" s="34"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="34">
+        <v>1</v>
+      </c>
+      <c r="P67" s="77">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="37"/>
-      <c r="L67" s="28">
-        <v>1</v>
-      </c>
-      <c r="M67" s="28">
-        <v>0</v>
-      </c>
-      <c r="N67" s="28"/>
-      <c r="O67" s="37"/>
-      <c r="P67" s="79">
-        <f t="shared" ref="P67" si="4">SUM(J67:M67)</f>
-        <v>1</v>
       </c>
       <c r="Q67" s="15"/>
       <c r="R67" s="3"/>
-      <c r="S67"/>
-      <c r="T67"/>
-      <c r="U67"/>
-      <c r="V67"/>
-      <c r="W67"/>
-      <c r="X67"/>
-      <c r="Y67"/>
-    </row>
-    <row r="68" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="11"/>
+    </row>
+    <row r="68" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="27">
+        <v>4</v>
+      </c>
+      <c r="D68" s="27">
+        <v>0</v>
+      </c>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="28">
+        <v>1</v>
+      </c>
+      <c r="M68" s="28">
+        <v>0</v>
+      </c>
+      <c r="N68" s="28"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="79">
+        <f t="shared" ref="P68" si="2">SUM(J68:M68)</f>
+        <v>1</v>
+      </c>
       <c r="Q68" s="15"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I69" s="64" t="s">
+      <c r="R68" s="3"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+    </row>
+    <row r="69" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="11"/>
+      <c r="Q69" s="15"/>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I70" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J69" s="85"/>
-      <c r="K69" s="85"/>
-      <c r="L69" s="65">
-        <f t="array" ref="L69">SUM($C2:$C67*(L2:L67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
+      <c r="J70" s="85"/>
+      <c r="K70" s="85"/>
+      <c r="L70" s="65">
+        <f t="array" ref="L70">SUM($C2:$C68*(L2:L68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
         <v>183</v>
       </c>
-      <c r="M69" s="65">
-        <f t="array" ref="M69">SUM($C2:$C67*(M2:M67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
+      <c r="M70" s="65">
+        <f t="array" ref="M70">SUM($C2:$C68*(M2:M68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
         <v>112</v>
       </c>
-      <c r="N69" s="65">
-        <f t="array" ref="N69">SUM($C2:$C67*(N2:N67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
+      <c r="N70" s="65">
+        <f t="array" ref="N70">SUM($C2:$C68*(N2:N68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
         <v>0</v>
       </c>
-      <c r="O69" s="66">
-        <f t="array" ref="O69">SUM($C2:$C67*(O2:O67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="Q69" s="15"/>
-      <c r="T69" s="33"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I70" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="J70" s="86"/>
-      <c r="K70" s="86"/>
-      <c r="L70" s="68">
-        <f t="array" ref="L70">SUM($C2:$C67*L2:L67*($P2:$P67&gt;=$R$12))</f>
-        <v>185.5</v>
-      </c>
-      <c r="M70" s="68">
-        <f t="array" ref="M70">SUM($C2:$C67*M2:M67*($P2:$P67&gt;=$R$12))</f>
-        <v>164.50000000000003</v>
-      </c>
-      <c r="N70" s="68">
-        <f t="array" ref="N70">SUM($C2:$C67*N2:N67*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="O70" s="69">
-        <f t="array" ref="O70">SUM($C2:$C67*O2:O67*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
+      <c r="O70" s="66">
+        <f t="array" ref="O70">SUM($C2:$C68*(O2:O68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
+        <v>209</v>
       </c>
       <c r="Q70" s="15"/>
-      <c r="V70" s="6"/>
-      <c r="W70" s="6"/>
-      <c r="X70" s="6"/>
-      <c r="Y70" s="6"/>
+      <c r="T70" s="33"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I71" s="67" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J71" s="86"/>
       <c r="K71" s="86"/>
       <c r="L71" s="68">
-        <f t="array" ref="L71">SUM($C$2:$C$67*(L$2:L$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>188</v>
+        <f t="array" ref="L71">SUM($C2:$C68*L2:L68*($P2:$P68&gt;=$R$12))</f>
+        <v>185.5</v>
       </c>
       <c r="M71" s="68">
-        <f t="array" ref="M71">SUM($C$2:$C$67*(M$2:M$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>198</v>
+        <f t="array" ref="M71">SUM($C2:$C68*M2:M68*($P2:$P68&gt;=$R$12))</f>
+        <v>164.50000000000003</v>
       </c>
       <c r="N71" s="68">
-        <f t="array" ref="N71">SUM($C$2:$C$67*(N$2:N$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
+        <f t="array" ref="N71">SUM($C2:$C68*N2:N68*($P2:$P68&gt;=$R$12))</f>
         <v>0</v>
       </c>
       <c r="O71" s="69">
-        <f t="array" ref="O71">SUM($C$2:$C$67*(O$2:O$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>0</v>
+        <f t="array" ref="O71">SUM($C2:$C68*O2:O68*($P2:$P68&gt;=$R$12))</f>
+        <v>209</v>
       </c>
       <c r="Q71" s="15"/>
-    </row>
-    <row r="72" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="6"/>
+      <c r="Y71" s="6"/>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I72" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J72" s="86"/>
       <c r="K72" s="86"/>
       <c r="L72" s="68">
+        <f t="array" ref="L72">SUM($C$2:$C$68*(L$2:L$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>188</v>
+      </c>
+      <c r="M72" s="68">
+        <f t="array" ref="M72">SUM($C$2:$C$68*(M$2:M$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>198</v>
+      </c>
+      <c r="N72" s="68">
+        <f t="array" ref="N72">SUM($C$2:$C$68*(N$2:N$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>0</v>
+      </c>
+      <c r="O72" s="69">
+        <f t="array" ref="O72">SUM($C$2:$C$68*(O$2:O$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>209</v>
+      </c>
+      <c r="Q72" s="15"/>
+    </row>
+    <row r="73" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="J73" s="86"/>
+      <c r="K73" s="86"/>
+      <c r="L73" s="68">
         <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>211</v>
       </c>
-      <c r="M72" s="68">
+      <c r="M73" s="68">
         <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>211</v>
       </c>
-      <c r="N72" s="68">
+      <c r="N73" s="68">
         <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>211</v>
       </c>
-      <c r="O72" s="69">
+      <c r="O73" s="69">
         <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>211</v>
       </c>
-      <c r="P72" s="3"/>
-      <c r="Q72" s="15"/>
-      <c r="R72" s="3"/>
-      <c r="S72"/>
-      <c r="T72"/>
-      <c r="U72"/>
-      <c r="V72"/>
-      <c r="W72"/>
-      <c r="X72"/>
-      <c r="Y72"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I73" s="67" t="s">
+      <c r="P73" s="3"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="3"/>
+      <c r="S73"/>
+      <c r="T73"/>
+      <c r="U73"/>
+      <c r="V73"/>
+      <c r="W73"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I74" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J73" s="86"/>
-      <c r="K73" s="86"/>
-      <c r="L73" s="70">
-        <f t="shared" ref="L73:O73" si="5">L70/L72</f>
+      <c r="J74" s="86"/>
+      <c r="K74" s="86"/>
+      <c r="L74" s="70">
+        <f t="shared" ref="L74:O74" si="3">L71/L73</f>
         <v>0.87914691943127965</v>
       </c>
-      <c r="M73" s="70">
-        <f t="shared" si="5"/>
+      <c r="M74" s="70">
+        <f t="shared" si="3"/>
         <v>0.77962085308056883</v>
       </c>
-      <c r="N73" s="70">
-        <f t="shared" si="5"/>
+      <c r="N74" s="70">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O73" s="71">
-        <f t="shared" si="5"/>
+      <c r="O74" s="71">
+        <f t="shared" si="3"/>
+        <v>0.99052132701421802</v>
+      </c>
+      <c r="Q74" s="15"/>
+      <c r="V74" s="6"/>
+      <c r="W74" s="6"/>
+      <c r="X74" s="6"/>
+      <c r="Y74" s="6"/>
+    </row>
+    <row r="75" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C75" s="33"/>
+      <c r="I75" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="J75" s="87"/>
+      <c r="K75" s="87"/>
+      <c r="L75" s="73">
+        <f t="array" ref="L75">SUM($C2:$C68*L2:L68*($P2:$P68&lt;$R$12))</f>
+        <v>10.5</v>
+      </c>
+      <c r="M75" s="73">
+        <f t="array" ref="M75">SUM($C2:$C68*M2:M68*($P2:$P68&lt;$R$12))</f>
+        <v>26.599999999999998</v>
+      </c>
+      <c r="N75" s="73">
+        <f t="array" ref="N75">SUM($C2:$C68*N2:N68*($P2:$P68&lt;$R$12))</f>
         <v>0</v>
       </c>
-      <c r="Q73" s="15"/>
-      <c r="V73" s="6"/>
-      <c r="W73" s="6"/>
-      <c r="X73" s="6"/>
-      <c r="Y73" s="6"/>
-    </row>
-    <row r="74" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C74" s="33"/>
-      <c r="I74" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="J74" s="87"/>
-      <c r="K74" s="87"/>
-      <c r="L74" s="73">
-        <f t="array" ref="L74">SUM($C2:$C67*L2:L67*($P2:$P67&lt;$R$12))</f>
-        <v>10.5</v>
-      </c>
-      <c r="M74" s="73">
-        <f t="array" ref="M74">SUM($C2:$C67*M2:M67*($P2:$P67&lt;$R$12))</f>
-        <v>26.599999999999998</v>
-      </c>
-      <c r="N74" s="73">
-        <f t="array" ref="N74">SUM($C2:$C67*N2:N67*($P2:$P67&lt;$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="O74" s="74">
-        <f t="array" ref="O74">SUM($C2:$C67*O2:O67*($P2:$P67&lt;$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="Q74" s="15"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C75" s="33"/>
+      <c r="O75" s="74">
+        <f t="array" ref="O75">SUM($C2:$C68*O2:O68*($P2:$P68&lt;$R$12))</f>
+        <v>9</v>
+      </c>
       <c r="Q75" s="15"/>
-      <c r="V75" s="6"/>
-      <c r="W75" s="6"/>
-      <c r="X75" s="6"/>
-      <c r="Y75" s="6"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C76" s="33"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
-      <c r="K76" s="14"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="14"/>
       <c r="Q76" s="15"/>
+      <c r="V76" s="6"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="6"/>
+      <c r="Y76" s="6"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C77" s="33"/>
@@ -4666,6 +4773,7 @@
       <c r="Q77" s="15"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C78" s="33"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
       <c r="K78" s="14"/>
@@ -4688,7 +4796,6 @@
       <c r="L80" s="14"/>
       <c r="M80" s="14"/>
       <c r="Q80" s="15"/>
-      <c r="U80" s="33"/>
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I81" s="14"/>
@@ -4697,6 +4804,7 @@
       <c r="L81" s="14"/>
       <c r="M81" s="14"/>
       <c r="Q81" s="15"/>
+      <c r="U81" s="33"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I82" s="14"/>
@@ -4704,6 +4812,7 @@
       <c r="K82" s="14"/>
       <c r="L82" s="14"/>
       <c r="M82" s="14"/>
+      <c r="Q82" s="15"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I83" s="14"/>
@@ -4712,59 +4821,66 @@
       <c r="L83" s="14"/>
       <c r="M83" s="14"/>
     </row>
-    <row r="85" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="10"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="20"/>
-      <c r="J85" s="36"/>
-      <c r="K85" s="36"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="20"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="3"/>
-      <c r="R85" s="3"/>
-      <c r="S85"/>
-      <c r="T85"/>
-      <c r="U85"/>
-      <c r="V85"/>
-      <c r="W85"/>
-      <c r="X85"/>
-      <c r="Y85"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="V88" s="6"/>
-      <c r="W88" s="6"/>
-      <c r="X88" s="6"/>
-      <c r="Y88" s="6"/>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="V92" s="6"/>
-      <c r="W92" s="6"/>
-      <c r="X92" s="6"/>
-      <c r="Y92" s="6"/>
-    </row>
-    <row r="97" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V97" s="6"/>
-      <c r="W97" s="6"/>
-      <c r="X97" s="6"/>
-      <c r="Y97" s="6"/>
-    </row>
-    <row r="110" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V110" s="33"/>
-      <c r="W110" s="33"/>
-      <c r="X110" s="33"/>
-      <c r="Y110" s="33"/>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+    </row>
+    <row r="86" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="10"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="20"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86"/>
+      <c r="T86"/>
+      <c r="U86"/>
+      <c r="V86"/>
+      <c r="W86"/>
+      <c r="X86"/>
+      <c r="Y86"/>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V89" s="6"/>
+      <c r="W89" s="6"/>
+      <c r="X89" s="6"/>
+      <c r="Y89" s="6"/>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V93" s="6"/>
+      <c r="W93" s="6"/>
+      <c r="X93" s="6"/>
+      <c r="Y93" s="6"/>
+    </row>
+    <row r="98" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V98" s="6"/>
+      <c r="W98" s="6"/>
+      <c r="X98" s="6"/>
+      <c r="Y98" s="6"/>
+    </row>
+    <row r="111" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V111" s="33"/>
+      <c r="W111" s="33"/>
+      <c r="X111" s="33"/>
+      <c r="Y111" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P67">
+  <conditionalFormatting sqref="B2:P68">
     <cfRule type="expression" dxfId="2" priority="31" stopIfTrue="1">
       <formula>$P2&gt;=(0.5+$R$12)</formula>
     </cfRule>

</xml_diff>